<commit_message>
graph month apple count
</commit_message>
<xml_diff>
--- a/dataGraphs.xlsx
+++ b/dataGraphs.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="20">
   <si>
     <t>Date</t>
   </si>
@@ -77,6 +77,9 @@
   </si>
   <si>
     <t>number</t>
+  </si>
+  <si>
+    <t>month</t>
   </si>
 </sst>
 </file>
@@ -3345,6 +3348,460 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
+          <c:x val="2.9775831863428442E-2"/>
+          <c:y val="1.7115848750039051E-2"/>
+          <c:w val="0.91168963567817141"/>
+          <c:h val="0.93201779484463565"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Samsung!$L$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>stock</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>Samsung!$L$2:$L$53</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="52"/>
+                <c:pt idx="0">
+                  <c:v>1360</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1350</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1387</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1350</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1370</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1395</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1415</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1468.75</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1470</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1350</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1398.75</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1413</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1379</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1375</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1367.7360000000001</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1405.8679999999999</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1335</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1321</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1402</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1400</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1400</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1208</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1140</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1146</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1188</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1192.8</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1200</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1132.22</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1075</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1075</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1174</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1258.25</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>1297</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>1342</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>1312</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1310</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>1374</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>1450</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>1450</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>1390</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>1370</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>1402</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>1400</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>1340</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>1356.25</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="329735552"/>
+        <c:axId val="331070464"/>
+      </c:lineChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Samsung!$K$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>rating</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>Samsung!$K$2:$K$53</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="52"/>
+                <c:pt idx="0">
+                  <c:v>3.9855072463768102</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.0294117647058796</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.2564102564102502</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.6279069767441801</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.88</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.4722222222222197</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.1818181818181799</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.95744680851063</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.4363636363636303</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.1111111111111098</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4.17777777777777</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.1224489795918302</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4.3953488372093004</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4.375</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4.57407407407407</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4.4444444444444402</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4.1884057971014403</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4.3250000000000002</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4.1372549019607803</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>4.5333333333333297</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>4.4047619047618998</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>4.1111111111111098</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>4.4901960784313699</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>4.3043478260869499</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>4.38</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>4.32</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>4.5434782608695601</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>4.2037037037036997</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>4.2758620689655098</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>4.3414634146341404</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>4.3250000000000002</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>4.5769230769230704</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>4.4090909090909003</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>4.5185185185185102</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>4.2222222222222197</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>4.4400000000000004</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>4.3913043478260798</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>4.5102040816326499</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>4.3684210526315699</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>4.21428571428571</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>4.54901960784313</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>4.3888888888888804</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>4.3770491803278597</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>4.5522388059701404</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>4.4637681159420204</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>4.1739130434782599</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>4.3396226415094299</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>4.3902439024390203</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>4.1034482758620596</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>4.1142857142857103</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>4.3076923076923004</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>4.3125</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="390629632"/>
+        <c:axId val="390627328"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="329735552"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="331070464"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="331070464"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="329735552"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="390627328"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="r"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="390629632"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:catAx>
+        <c:axId val="390629632"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="none"/>
+        <c:crossAx val="390627328"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="pt-PT"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
           <c:x val="1.9976247307328165E-2"/>
           <c:y val="1.347002624671916E-2"/>
           <c:w val="0.92451000021196716"/>
@@ -3752,7 +4209,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="pt-PT"/>
   <c:chart>
@@ -9602,6 +10059,122 @@
   <c:lang val="pt-PT"/>
   <c:chart>
     <c:title>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Apple!$R$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>month</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>Apple!$R$2:$R$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>2695</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2099</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2179</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1878</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2022</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2008</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2200</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2196</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1738</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1916</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1956</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2902</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="378027392"/>
+        <c:axId val="378057472"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="378027392"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="378057472"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="378057472"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="378027392"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="pt-PT"/>
+  <c:chart>
+    <c:title>
       <c:tx>
         <c:rich>
           <a:bodyPr/>
@@ -10068,7 +10641,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="pt-PT"/>
   <c:chart>
@@ -10475,7 +11048,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="pt-PT"/>
   <c:chart>
@@ -10616,7 +11189,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="pt-PT"/>
   <c:chart>
@@ -10742,460 +11315,6 @@
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="pt-PT"/>
-  <c:chart>
-    <c:plotArea>
-      <c:layout>
-        <c:manualLayout>
-          <c:layoutTarget val="inner"/>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="2.9775831863428442E-2"/>
-          <c:y val="1.7115848750039051E-2"/>
-          <c:w val="0.91168963567817141"/>
-          <c:h val="0.93201779484463565"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Samsung!$L$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>stock</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:val>
-            <c:numRef>
-              <c:f>Samsung!$L$2:$L$53</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="52"/>
-                <c:pt idx="0">
-                  <c:v>1360</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1350</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1387</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1350</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1370</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1395</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1415</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1468.75</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1500</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1500</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1470</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1350</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1398.75</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1413</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>1379</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>1375</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>1300</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>1367.7360000000001</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>1405.8679999999999</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>1335</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>1321</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>1300</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>1402</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>1400</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>1400</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>1208</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>1140</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>1146</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>1188</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>1192.8</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>1200</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>1132.22</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>1075</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>1075</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>1174</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>1258.25</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>1297</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>1342</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>1300</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>1312</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>1310</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>1374</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>1450</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>1450</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>1390</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>1370</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>1402</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>1400</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>1340</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>1300</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>1300</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>1356.25</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:marker val="1"/>
-        <c:axId val="329735552"/>
-        <c:axId val="331070464"/>
-      </c:lineChart>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Samsung!$K$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>rating</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:val>
-            <c:numRef>
-              <c:f>Samsung!$K$2:$K$53</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="52"/>
-                <c:pt idx="0">
-                  <c:v>3.9855072463768102</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4.0294117647058796</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4.2564102564102502</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4.6279069767441801</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>3.88</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>4.4722222222222197</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>4.1818181818181799</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>3.95744680851063</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>4.4363636363636303</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>4.1111111111111098</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>4.17777777777777</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>4.1224489795918302</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>4.3953488372093004</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>4.375</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>4.57407407407407</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>4.4444444444444402</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>4.1884057971014403</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>4.3250000000000002</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>4.1372549019607803</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>4.5333333333333297</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>4.4047619047618998</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>4.1111111111111098</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>4.4901960784313699</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>4.3043478260869499</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>4.38</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>4.32</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>4.5434782608695601</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>4.2037037037036997</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>4.2758620689655098</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>4.3414634146341404</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>4.3250000000000002</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>4.5769230769230704</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>4.4090909090909003</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>4.5185185185185102</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>4.2222222222222197</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>4.4400000000000004</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>4.3913043478260798</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>4.5102040816326499</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>4.3684210526315699</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>4.21428571428571</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>4.54901960784313</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>4.3888888888888804</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>4.3770491803278597</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>4.5522388059701404</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>4.4637681159420204</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>4.1739130434782599</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>4.3396226415094299</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>4.3902439024390203</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>4.1034482758620596</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>4.1142857142857103</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>4.3076923076923004</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>4.3125</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:marker val="1"/>
-        <c:axId val="390629632"/>
-        <c:axId val="390627328"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="329735552"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:axPos val="b"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="331070464"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="331070464"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="329735552"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="390627328"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:axPos val="r"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="390629632"/>
-        <c:crosses val="max"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:catAx>
-        <c:axId val="390629632"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="1"/>
-        <c:axPos val="b"/>
-        <c:tickLblPos val="none"/>
-        <c:crossAx val="390627328"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-      </c:catAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
@@ -11337,6 +11456,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>217714</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>68036</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>571499</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name="Gráfico 8"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -11850,10 +11999,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O501"/>
+  <dimension ref="A1:R501"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1:O53"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="R1" sqref="R1:R13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -11869,7 +12018,7 @@
     <col min="12" max="12" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:18">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -11888,8 +12037,14 @@
       <c r="O1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:15">
+      <c r="Q1" t="s">
+        <v>19</v>
+      </c>
+      <c r="R1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18">
       <c r="A2" s="1">
         <v>41276</v>
       </c>
@@ -11923,8 +12078,14 @@
       <c r="O2">
         <v>837</v>
       </c>
-    </row>
-    <row r="3" spans="1:15">
+      <c r="Q2">
+        <v>1</v>
+      </c>
+      <c r="R2">
+        <v>2695</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18">
       <c r="A3" s="1">
         <v>41277</v>
       </c>
@@ -11965,8 +12126,14 @@
       <c r="O3">
         <v>633</v>
       </c>
-    </row>
-    <row r="4" spans="1:15">
+      <c r="Q3">
+        <v>2</v>
+      </c>
+      <c r="R3">
+        <v>2099</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18">
       <c r="A4" s="1">
         <v>41278</v>
       </c>
@@ -12007,8 +12174,14 @@
       <c r="O4">
         <v>585</v>
       </c>
-    </row>
-    <row r="5" spans="1:15">
+      <c r="Q4">
+        <v>3</v>
+      </c>
+      <c r="R4">
+        <v>2179</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18">
       <c r="A5" s="1">
         <v>41281</v>
       </c>
@@ -12038,8 +12211,14 @@
       <c r="O5">
         <v>566</v>
       </c>
-    </row>
-    <row r="6" spans="1:15">
+      <c r="Q5">
+        <v>4</v>
+      </c>
+      <c r="R5">
+        <v>1878</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18">
       <c r="A6" s="1">
         <v>41282</v>
       </c>
@@ -12069,8 +12248,14 @@
       <c r="O6">
         <v>622</v>
       </c>
-    </row>
-    <row r="7" spans="1:15">
+      <c r="Q6">
+        <v>5</v>
+      </c>
+      <c r="R6">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18">
       <c r="A7" s="1">
         <v>41283</v>
       </c>
@@ -12100,8 +12285,14 @@
       <c r="O7">
         <v>548</v>
       </c>
-    </row>
-    <row r="8" spans="1:15">
+      <c r="Q7">
+        <v>6</v>
+      </c>
+      <c r="R7">
+        <v>2008</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18">
       <c r="A8" s="1">
         <v>41284</v>
       </c>
@@ -12131,8 +12322,14 @@
       <c r="O8">
         <v>454</v>
       </c>
-    </row>
-    <row r="9" spans="1:15">
+      <c r="Q8">
+        <v>7</v>
+      </c>
+      <c r="R8">
+        <v>2200</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18">
       <c r="A9" s="1">
         <v>41285</v>
       </c>
@@ -12162,8 +12359,14 @@
       <c r="O9">
         <v>549</v>
       </c>
-    </row>
-    <row r="10" spans="1:15">
+      <c r="Q9">
+        <v>8</v>
+      </c>
+      <c r="R9">
+        <v>2196</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18">
       <c r="A10" s="1">
         <v>41288</v>
       </c>
@@ -12193,8 +12396,14 @@
       <c r="O10">
         <v>546</v>
       </c>
-    </row>
-    <row r="11" spans="1:15">
+      <c r="Q10">
+        <v>9</v>
+      </c>
+      <c r="R10">
+        <v>1738</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18">
       <c r="A11" s="1">
         <v>41289</v>
       </c>
@@ -12224,8 +12433,14 @@
       <c r="O11">
         <v>549</v>
       </c>
-    </row>
-    <row r="12" spans="1:15">
+      <c r="Q11">
+        <v>10</v>
+      </c>
+      <c r="R11">
+        <v>1916</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18">
       <c r="A12" s="1">
         <v>41290</v>
       </c>
@@ -12255,8 +12470,14 @@
       <c r="O12">
         <v>452</v>
       </c>
-    </row>
-    <row r="13" spans="1:15">
+      <c r="Q12">
+        <v>11</v>
+      </c>
+      <c r="R12">
+        <v>1956</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18">
       <c r="A13" s="1">
         <v>41291</v>
       </c>
@@ -12286,8 +12507,14 @@
       <c r="O13">
         <v>468</v>
       </c>
-    </row>
-    <row r="14" spans="1:15">
+      <c r="Q13">
+        <v>12</v>
+      </c>
+      <c r="R13">
+        <v>2902</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18">
       <c r="A14" s="1">
         <v>41292</v>
       </c>
@@ -12318,7 +12545,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="15" spans="1:15">
+    <row r="15" spans="1:18">
       <c r="A15" s="1">
         <v>41296</v>
       </c>
@@ -12349,7 +12576,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="16" spans="1:15">
+    <row r="16" spans="1:18">
       <c r="A16" s="1">
         <v>41297</v>
       </c>

</xml_diff>